<commit_message>
feat: remove pandas and use parser module instead
</commit_message>
<xml_diff>
--- a/mothertongues/tests/data/data.xlsx
+++ b/mothertongues/tests/data/data.xlsx
@@ -1,22 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10312"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10409"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/pinea/mtd/mothertongues/tests/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B094F840-5880-C94A-B53A-626FC66E9FE5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BCB2056E-EB2B-8342-9B69-5592544A501E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11580" yWindow="5400" windowWidth="28040" windowHeight="17440" xr2:uid="{941A79BD-FFFA-C248-99DE-551C3B456D9A}"/>
+    <workbookView xWindow="10360" yWindow="2480" windowWidth="28040" windowHeight="17440" xr2:uid="{941A79BD-FFFA-C248-99DE-551C3B456D9A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Skip" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
     <definedName name="data" localSheetId="0">Sheet1!$A$1:$G$4</definedName>
+    <definedName name="data_1" localSheetId="1">Skip!$A$2:$G$5</definedName>
   </definedNames>
   <calcPr calcId="181029"/>
   <extLst>
@@ -53,11 +55,24 @@
       </textFields>
     </textPr>
   </connection>
+  <connection id="2" xr16:uid="{90861447-7349-8B4C-A1B2-BF4FF80224AF}" name="data1" type="6" refreshedVersion="8" background="1" saveData="1">
+    <textPr sourceFile="/Users/pinea/mtd/mothertongues/tests/data/data.csv" comma="1">
+      <textFields count="7">
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+      </textFields>
+    </textPr>
+  </connection>
 </connections>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="23">
   <si>
     <t>tree</t>
   </si>
@@ -108,6 +123,24 @@
   </si>
   <si>
     <t>træ</t>
+  </si>
+  <si>
+    <t>ID</t>
+  </si>
+  <si>
+    <t>definition</t>
+  </si>
+  <si>
+    <t>audio_desc</t>
+  </si>
+  <si>
+    <t>audio_fn</t>
+  </si>
+  <si>
+    <t>theme</t>
+  </si>
+  <si>
+    <t>secondary_theme</t>
   </si>
 </sst>
 </file>
@@ -164,6 +197,10 @@
 
 <file path=xl/queryTables/queryTable1.xml><?xml version="1.0" encoding="utf-8"?>
 <queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="data" connectionId="1" xr16:uid="{7B027112-F929-EF4E-A321-EEEBECE38E7E}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable2.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="data_1" connectionId="2" xr16:uid="{BB2DC2E0-2ACB-D448-89EC-7544871D6C7F}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -466,7 +503,7 @@
   <dimension ref="A1:G4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -569,4 +606,128 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2BF3A8DC-86E6-E245-AEFF-D52BAA8E1CC1}">
+  <dimension ref="A1:G5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E1" t="s">
+        <v>20</v>
+      </c>
+      <c r="F1" t="s">
+        <v>21</v>
+      </c>
+      <c r="G1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D2" t="s">
+        <v>1</v>
+      </c>
+      <c r="E2" t="s">
+        <v>2</v>
+      </c>
+      <c r="F2" t="s">
+        <v>3</v>
+      </c>
+      <c r="G2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D3" t="s">
+        <v>1</v>
+      </c>
+      <c r="E3" t="s">
+        <v>7</v>
+      </c>
+      <c r="F3" t="s">
+        <v>8</v>
+      </c>
+      <c r="G3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4" t="s">
+        <v>10</v>
+      </c>
+      <c r="D4" t="s">
+        <v>1</v>
+      </c>
+      <c r="E4" t="s">
+        <v>11</v>
+      </c>
+      <c r="F4" t="s">
+        <v>12</v>
+      </c>
+      <c r="G4" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>14</v>
+      </c>
+      <c r="C5" t="s">
+        <v>15</v>
+      </c>
+      <c r="F5" t="s">
+        <v>12</v>
+      </c>
+      <c r="G5" t="s">
+        <v>13</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
feat: add video to dictionary entry format
</commit_message>
<xml_diff>
--- a/mothertongues/tests/data/data.xlsx
+++ b/mothertongues/tests/data/data.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10409"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10114"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/pinea/mtd/mothertongues/tests/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nolanvanhell/github/mothertongues/mothertongues/tests/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BCB2056E-EB2B-8342-9B69-5592544A501E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46F0FBAC-A4E6-8844-8BFE-492938D72A00}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="10360" yWindow="2480" windowWidth="28040" windowHeight="17440" xr2:uid="{941A79BD-FFFA-C248-99DE-551C3B456D9A}"/>
   </bookViews>
@@ -17,8 +17,8 @@
     <sheet name="Skip" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="data" localSheetId="0">Sheet1!$A$1:$G$4</definedName>
-    <definedName name="data_1" localSheetId="1">Skip!$A$2:$G$5</definedName>
+    <definedName name="data" localSheetId="0">Sheet1!$A$1:$I$4</definedName>
+    <definedName name="data_1" localSheetId="1">Skip!$A$2:$I$5</definedName>
   </definedNames>
   <calcPr calcId="181029"/>
   <extLst>
@@ -72,7 +72,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="27">
   <si>
     <t>tree</t>
   </si>
@@ -141,16 +141,34 @@
   </si>
   <si>
     <t>secondary_theme</t>
+  </si>
+  <si>
+    <t>Nolan Van Hell</t>
+  </si>
+  <si>
+    <t>snowfall.mp4</t>
+  </si>
+  <si>
+    <t>video_desc</t>
+  </si>
+  <si>
+    <t>video_fn</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -500,10 +518,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{88BD1A24-287F-A749-8A9B-42DE365BE9F1}">
-  <dimension ref="A1:G4"/>
+  <dimension ref="A1:I4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -513,11 +531,13 @@
     <col min="3" max="3" width="5.83203125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="9.83203125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="8.6640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="8.83203125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="8.83203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1">
         <v>1</v>
       </c>
@@ -534,13 +554,19 @@
         <v>2</v>
       </c>
       <c r="F1" t="s">
+        <v>23</v>
+      </c>
+      <c r="G1" t="s">
+        <v>24</v>
+      </c>
+      <c r="H1" t="s">
         <v>3</v>
       </c>
-      <c r="G1" t="s">
+      <c r="I1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>2</v>
       </c>
@@ -557,13 +583,19 @@
         <v>7</v>
       </c>
       <c r="F2" t="s">
+        <v>23</v>
+      </c>
+      <c r="G2" t="s">
+        <v>24</v>
+      </c>
+      <c r="H2" t="s">
         <v>8</v>
       </c>
-      <c r="G2" t="s">
+      <c r="I2" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>3</v>
       </c>
@@ -580,13 +612,19 @@
         <v>11</v>
       </c>
       <c r="F3" t="s">
+        <v>23</v>
+      </c>
+      <c r="G3" t="s">
+        <v>24</v>
+      </c>
+      <c r="H3" t="s">
         <v>12</v>
       </c>
-      <c r="G3" t="s">
+      <c r="I3" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>4</v>
       </c>
@@ -596,29 +634,34 @@
       <c r="C4" t="s">
         <v>15</v>
       </c>
-      <c r="F4" t="s">
+      <c r="H4" t="s">
         <v>12</v>
       </c>
-      <c r="G4" t="s">
+      <c r="I4" t="s">
         <v>13</v>
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2BF3A8DC-86E6-E245-AEFF-D52BAA8E1CC1}">
-  <dimension ref="A1:G5"/>
+  <dimension ref="A1:I5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="6" max="6" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.33203125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>17</v>
       </c>
@@ -635,13 +678,19 @@
         <v>20</v>
       </c>
       <c r="F1" t="s">
+        <v>25</v>
+      </c>
+      <c r="G1" t="s">
+        <v>26</v>
+      </c>
+      <c r="H1" t="s">
         <v>21</v>
       </c>
-      <c r="G1" t="s">
+      <c r="I1" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
@@ -658,13 +707,19 @@
         <v>2</v>
       </c>
       <c r="F2" t="s">
+        <v>23</v>
+      </c>
+      <c r="G2" t="s">
+        <v>24</v>
+      </c>
+      <c r="H2" t="s">
         <v>3</v>
       </c>
-      <c r="G2" t="s">
+      <c r="I2" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>2</v>
       </c>
@@ -681,13 +736,19 @@
         <v>7</v>
       </c>
       <c r="F3" t="s">
+        <v>23</v>
+      </c>
+      <c r="G3" t="s">
+        <v>24</v>
+      </c>
+      <c r="H3" t="s">
         <v>8</v>
       </c>
-      <c r="G3" t="s">
+      <c r="I3" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>3</v>
       </c>
@@ -704,13 +765,19 @@
         <v>11</v>
       </c>
       <c r="F4" t="s">
+        <v>23</v>
+      </c>
+      <c r="G4" t="s">
+        <v>24</v>
+      </c>
+      <c r="H4" t="s">
         <v>12</v>
       </c>
-      <c r="G4" t="s">
+      <c r="I4" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>4</v>
       </c>
@@ -720,14 +787,15 @@
       <c r="C5" t="s">
         <v>15</v>
       </c>
-      <c r="F5" t="s">
+      <c r="H5" t="s">
         <v>12</v>
       </c>
-      <c r="G5" t="s">
+      <c r="I5" t="s">
         <v>13</v>
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>